<commit_message>
v1.1 close the previous status
close the previous status and add more comments
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_USERHOME_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_USERHOME_REVIEWS.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\TCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId1"/>
+    <sheet name="LH-TC-USERHOME-Reviews" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Author</t>
   </si>
@@ -78,6 +78,12 @@
     <t>Reviewed Entity</t>
   </si>
   <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
     <t>13/5/2025</t>
   </si>
   <si>
@@ -87,6 +93,9 @@
     <t>Open</t>
   </si>
   <si>
+    <t>review  the user home feature test cases</t>
+  </si>
+  <si>
     <t>LH_TC_USERHOME_REVIEW_001</t>
   </si>
   <si>
@@ -129,19 +138,22 @@
     <t>please modify the formate the font size and type</t>
   </si>
   <si>
-    <t>Hala Eldaly</t>
-  </si>
-  <si>
-    <t>Review  the user home feature test cases</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Close owner status</t>
+    <t>LH_TC_USERHOME_REVIEW_004</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>ia all data you mention that there is a correct password but this password doesn't match acceptance criteria of the password</t>
+  </si>
+  <si>
+    <t>so please make the password valid something like that "CorrectPassword@123"</t>
+  </si>
+  <si>
+    <t>14/5/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">close the previous status and add more comments </t>
   </si>
 </sst>
 </file>
@@ -272,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -323,9 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,7 +774,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="Version Number" dataDxfId="3"/>
     <tableColumn id="2" name="Author" dataDxfId="2"/>
@@ -1075,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="B1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1128,107 +1137,125 @@
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="7"/>
+      <c r="J5" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
@@ -1303,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,27 +1361,27 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.2 close user home review
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_USERHOME_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_USERHOME_REVIEWS.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Author</t>
   </si>
@@ -90,7 +90,7 @@
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>v1.2</t>
   </si>
   <si>
     <t>review  the user home feature test cases</t>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t xml:space="preserve">close the previous status and add more comments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">close user home review </t>
   </si>
 </sst>
 </file>
@@ -774,7 +777,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
     <tableColumn id="1" name="Version Number" dataDxfId="3"/>
     <tableColumn id="2" name="Author" dataDxfId="2"/>
@@ -1085,7 +1088,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1251,10 +1254,10 @@
         <v>25</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1328,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1387,20 @@
         <v>38</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>